<commit_message>
create demo sheet from local notebook functions.
</commit_message>
<xml_diff>
--- a/src/taskpane/utils/demo_sheet.xlsx
+++ b/src/taskpane/utils/demo_sheet.xlsx
@@ -8,15 +8,19 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\brent\Code\python\src\taskpane\utils\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B1EC8E37-DAE1-47DD-ABAB-3F5E4F3F3C89}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0FB00A71-BE98-4A17-B466-1D16CF128428}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="16220" xr2:uid="{250729AF-73FD-4BBC-A738-7E40FF49336E}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="DemoFunctions" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="HELLO" comment="Returns a greeting">_xlfn.LAMBDA(_xlpm.name, _xldudf_LOCAL_EXEC("workbook-settings:hello", _xlpm.name))</definedName>
+    <definedName name="ADD_TWO_DAYS" comment="Add two days to the given date">_xlfn.LAMBDA(_xlpm.date_input, _xldudf_LOCAL_EXEC("workbook-settings:add_two_days", _xlpm.date_input))</definedName>
+    <definedName name="CALCULATE_AREA" comment="Calculate area of rectangle">_xlfn.LAMBDA(_xlpm.length,_xlpm.width, _xldudf_LOCAL_EXEC("workbook-settings:calculate_area", _xlpm.length, _xlpm.width))</definedName>
+    <definedName name="IN_RANGE" comment="Check if number is in range [min_val, max_val]">_xlfn.LAMBDA(_xlpm.number,_xlpm.min_val,_xlpm.max_val, _xldudf_LOCAL_EXEC("workbook-settings:in_range", _xlpm.number, _xlpm.min_val, _xlpm.max_val))</definedName>
+    <definedName name="JOIN_STRINGS" comment="Join two strings with a separator">_xlfn.LAMBDA(_xlpm.first_str,_xlpm.second_str,_xlpm.separator, _xldudf_LOCAL_EXEC("workbook-settings:join_strings", _xlpm.first_str, _xlpm.second_str, _xlpm.separator))</definedName>
+    <definedName name="TO_POWER" comment="Calculate power with rounding">_xlfn.LAMBDA(_xlpm.base,_xlpm.exponent,_xlpm.round_to, _xldudf_LOCAL_EXEC("workbook-settings:to_power", _xlpm.base, _xlpm.exponent, _xlpm.round_to))</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -435,7 +439,7 @@
 
 <file path=xl/webextensions/taskpanes.xml><?xml version="1.0" encoding="utf-8"?>
 <wetp:taskpanes xmlns:wetp="http://schemas.microsoft.com/office/webextensions/taskpanes/2010/11">
-  <wetp:taskpane dockstate="right" visibility="0" width="525" row="8">
+  <wetp:taskpane dockstate="right" visibility="0" width="621" row="8">
     <wetp:webextensionref xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
   </wetp:taskpane>
 </wetp:taskpanes>
@@ -446,11 +450,18 @@
   <we:reference id="b991da66-1687-44ee-8d65-61ab1dfd8b0f" version="1.0.0.0" store="developer" storeType="Registry"/>
   <we:alternateReferences/>
   <we:properties>
-    <we:property name="hello" value="{&quot;name&quot;:&quot;hello&quot;,&quot;signature&quot;:&quot;HELLO(name)&quot;,&quot;description&quot;:&quot;Returns a greeting&quot;,&quot;code&quot;:&quot;def hello(name):\n    \&quot;\&quot;\&quot; Returns a greeting. \&quot;\&quot;\&quot;\n    return f\&quot;Hello {name}!\&quot;\n    \n# Arguments to test the function.\ntest_cases = [\n    [\&quot;Nancy\&quot;],\n    [\&quot;Ming\&quot;]\n]&quot;,&quot;resultLine&quot;:&quot;\n\nresult = hello(arg1)&quot;,&quot;formula&quot;:&quot;=LAMBDA(name, LOCAL.EXEC(\&quot;workbook-settings:hello\&quot;, name))&quot;,&quot;timestamp&quot;:&quot;2025-02-09T21:32:53.824Z&quot;,&quot;uid&quot;:&quot;anonymous&quot;,&quot;excelExample&quot;:null}"/>
+    <we:property name="calculate_area" value="{&quot;name&quot;:&quot;calculate_area&quot;,&quot;signature&quot;:&quot;CALCULATE_AREA(length, width)&quot;,&quot;description&quot;:&quot;Calculate area of rectangle&quot;,&quot;code&quot;:&quot;def calculate_area(length, width):\n    \&quot;\&quot;\&quot;Calculate area of rectangle.\n    Args:\n        length (float): Length of rectangle\n        width (float): Width of rectangle\n    Returns:\n        float: Area of rectangle\n    \&quot;\&quot;\&quot;\n    return length * width\n\ntest_cases = [\n    [5, 4],      # -&gt; 20\n    [2.5, 4],    # -&gt; 10\n    [10, 10],    # -&gt; 100\n    [1, 1],      # -&gt; 1\n    [0.5, 2]     # -&gt; 1\n]\n\n# Excel usage: =CALCULATE_AREA(5, 4)&quot;,&quot;resultLine&quot;:&quot;\n\nresult = calculate_area(arg1, arg2)&quot;,&quot;formula&quot;:&quot;=LAMBDA(length, width, LOCAL.EXEC(\&quot;workbook-settings:calculate_area\&quot;, length, width))&quot;,&quot;timestamp&quot;:&quot;2025-02-10T19:05:24.194Z&quot;,&quot;uid&quot;:&quot;anonymous&quot;,&quot;excelExample&quot;:&quot;=CALCULATE_AREA(5, 4)&quot;}"/>
+    <we:property name="join_strings" value="{&quot;name&quot;:&quot;join_strings&quot;,&quot;signature&quot;:&quot;JOIN_STRINGS(first_str, second_str, separator)&quot;,&quot;description&quot;:&quot;Join two strings with a separator&quot;,&quot;code&quot;:&quot;def join_strings(first_str, second_str, separator):\n    \&quot;\&quot;\&quot;Join two strings with a separator.\n    Args:\n        first_str (str): First string\n        second_str (str): Second string\n        separator (str): Separator between strings\n    Returns:\n        str: Joined string\n    \&quot;\&quot;\&quot;\n    return f\&quot;{first_str}{separator}{second_str}\&quot;\n\ntest_cases = [\n    [\&quot;hello\&quot;, \&quot;world\&quot;, \&quot; \&quot;],      # -&gt; \&quot;hello world\&quot;\n    [\&quot;first\&quot;, \&quot;last\&quot;, \&quot;-\&quot;],       # -&gt; \&quot;first-last\&quot;\n    [\&quot;a\&quot;, \&quot;b\&quot;, \&quot;_\&quot;],             # -&gt; \&quot;a_b\&quot;\n    [\&quot;python\&quot;, \&quot;code\&quot;, \&quot;::\&quot;],     # -&gt; \&quot;python::code\&quot;\n    [\&quot;x\&quot;, \&quot;y\&quot;, \&quot;\&quot;]               # -&gt; \&quot;xy\&quot;\n]\n\n# Excel usage: =JOIN_STRINGS(\&quot;hello\&quot;, \&quot;world\&quot;, \&quot; \&quot;)&quot;,&quot;resultLine&quot;:&quot;\n\nresult = join_strings(arg1, arg2, arg3)&quot;,&quot;formula&quot;:&quot;=LAMBDA(first_str, second_str, separator, LOCAL.EXEC(\&quot;workbook-settings:join_strings\&quot;, first_str, second_str, separator))&quot;,&quot;timestamp&quot;:&quot;2025-02-10T19:05:24.258Z&quot;,&quot;uid&quot;:&quot;anonymous&quot;,&quot;excelExample&quot;:&quot;=JOIN_STRINGS(\&quot;hello\&quot;, \&quot;world\&quot;, \&quot; \&quot;)&quot;}"/>
+    <we:property name="in_range" value="{&quot;name&quot;:&quot;in_range&quot;,&quot;signature&quot;:&quot;IN_RANGE(number, min_val, max_val)&quot;,&quot;description&quot;:&quot;Check if number is in range [min_val, max_val]&quot;,&quot;code&quot;:&quot;def in_range(number, min_val, max_val):\n    \&quot;\&quot;\&quot;Check if number is in range [min_val, max_val].\n    Args:\n        number (float): Number to check\n        min_val (float): Minimum value\n        max_val (float): Maximum value\n    Returns:\n        bool: True if in range, False otherwise\n    \&quot;\&quot;\&quot;\n    return min_val &lt;= number &lt;= max_val\n\ntest_cases = [\n    [5, 0, 10],       # -&gt; True\n    [-1, 0, 100],     # -&gt; False\n    [50, 50, 50],     # -&gt; True\n    [25, 0, 20],      # -&gt; False\n    [3.14, 3, 4]      # -&gt; True\n]\n\n# Excel usage: =IN_RANGE(5, 0, 10)&quot;,&quot;resultLine&quot;:&quot;\n\nresult = in_range(arg1, arg2, arg3)&quot;,&quot;formula&quot;:&quot;=LAMBDA(number, min_val, max_val, LOCAL.EXEC(\&quot;workbook-settings:in_range\&quot;, number, min_val, max_val))&quot;,&quot;timestamp&quot;:&quot;2025-02-10T19:05:24.318Z&quot;,&quot;uid&quot;:&quot;anonymous&quot;,&quot;excelExample&quot;:&quot;=IN_RANGE(5, 0, 10)&quot;}"/>
+    <we:property name="to_power" value="{&quot;name&quot;:&quot;to_power&quot;,&quot;signature&quot;:&quot;TO_POWER(base, exponent, round_to)&quot;,&quot;description&quot;:&quot;Calculate power with rounding&quot;,&quot;code&quot;:&quot;def to_power(base, exponent, round_to):\n    \&quot;\&quot;\&quot;Calculate power with rounding.\n    Args:\n        base (float): Base number\n        exponent (float): Exponent\n        round_to (int): Decimal places to round to\n    Returns:\n        float: Result rounded to specified decimals\n    \&quot;\&quot;\&quot;\n    return round(base ** exponent, round_to)\n\ntest_cases = [\n    [2, 3, 0],        # -&gt; 8\n    [5, 2, 1],        # -&gt; 25.0\n    [3, 0.5, 2],      # -&gt; 1.73\n    [10, -1, 3],      # -&gt; 0.100\n    [2.5, 2, 2]       # -&gt; 6.25\n]\n\n# Excel usage: =TO_POWER(2, 3, 0)&quot;,&quot;resultLine&quot;:&quot;\n\nresult = to_power(arg1, arg2, arg3)&quot;,&quot;formula&quot;:&quot;=LAMBDA(base, exponent, round_to, LOCAL.EXEC(\&quot;workbook-settings:to_power\&quot;, base, exponent, round_to))&quot;,&quot;timestamp&quot;:&quot;2025-02-10T19:05:24.376Z&quot;,&quot;uid&quot;:&quot;anonymous&quot;,&quot;excelExample&quot;:&quot;=TO_POWER(2, 3, 0)&quot;}"/>
+    <we:property name="add_two_days" value="{&quot;name&quot;:&quot;add_two_days&quot;,&quot;signature&quot;:&quot;ADD_TWO_DAYS(date_input)&quot;,&quot;description&quot;:&quot;Add two days to the given date&quot;,&quot;code&quot;:&quot;def add_two_days(date_input):\n    \&quot;\&quot;\&quot;Add two days to the given date.\n    Args:\n        date_input (str or int): Date in 'YYYY-MM-DD' format or Excel serial date\n    Returns:\n        str: New date in 'YYYY-MM-DD' format\n    \&quot;\&quot;\&quot;\n    from datetime import datetime, timedelta\n    \n    if isinstance(date_input, int):\n        # Excel serial date to datetime conversion\n        date = datetime(1899, 12, 30) + timedelta(days=date_input)\n    else:\n        date = datetime.strptime(date_input, '%Y-%m-%d')\n    \n    new_date = date + timedelta(days=2)\n    return new_date.strftime('%Y-%m-%d')\n\ntest_cases = [\n    [43831],\n    [44561],\n    ['2024-06-15'],\n    ['2025-01-01']\n]\n\n# Excel usage: =ADD_TWO_DAYS(43831)&quot;,&quot;resultLine&quot;:&quot;\n\nresult = add_two_days(arg1)&quot;,&quot;formula&quot;:&quot;=LAMBDA(date_input, LOCAL.EXEC(\&quot;workbook-settings:add_two_days\&quot;, date_input))&quot;,&quot;timestamp&quot;:&quot;2025-02-10T19:05:24.436Z&quot;,&quot;uid&quot;:&quot;anonymous&quot;,&quot;excelExample&quot;:&quot;=ADD_TWO_DAYS(43831)&quot;}"/>
   </we:properties>
   <we:bindings/>
   <we:snapshot xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships"/>
   <we:extLst>
+    <a:ext xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" uri="{D87F86FE-615C-45B5-9D79-34F1136793EB}">
+      <we:containsCustomFunctions val="1"/>
+    </a:ext>
     <a:ext xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" uri="{7C84B067-C214-45C3-A712-C9D94CD141B2}">
       <we:customFunctionIdList>
         <we:customFunctionIds>_xldudf_LOCAL_RUNPY</we:customFunctionIds>
@@ -466,7 +477,7 @@
   <dimension ref="B2:B4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D16" sqref="D16"/>
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -480,9 +491,9 @@
       </c>
     </row>
     <row r="4" spans="2:2" x14ac:dyDescent="0.35">
-      <c r="B4" t="str" cm="1">
-        <f t="array" ref="B4">HELLO("foo")</f>
-        <v>Hello foo!</v>
+      <c r="B4" cm="1">
+        <f t="array" ref="B4">CALCULATE_AREA(2,3)</f>
+        <v>6</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
add functions to settings and name manager after inserting demo sheet
</commit_message>
<xml_diff>
--- a/src/taskpane/utils/demo_sheet.xlsx
+++ b/src/taskpane/utils/demo_sheet.xlsx
@@ -8,20 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\brent\Code\python\src\taskpane\utils\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0FB00A71-BE98-4A17-B466-1D16CF128428}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B4A6D8BB-0E2B-45AB-9CED-5BB807BFE7C9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="16220" xr2:uid="{250729AF-73FD-4BBC-A738-7E40FF49336E}"/>
   </bookViews>
   <sheets>
     <sheet name="DemoFunctions" sheetId="1" r:id="rId1"/>
   </sheets>
-  <definedNames>
-    <definedName name="ADD_TWO_DAYS" comment="Add two days to the given date">_xlfn.LAMBDA(_xlpm.date_input, _xldudf_LOCAL_EXEC("workbook-settings:add_two_days", _xlpm.date_input))</definedName>
-    <definedName name="CALCULATE_AREA" comment="Calculate area of rectangle">_xlfn.LAMBDA(_xlpm.length,_xlpm.width, _xldudf_LOCAL_EXEC("workbook-settings:calculate_area", _xlpm.length, _xlpm.width))</definedName>
-    <definedName name="IN_RANGE" comment="Check if number is in range [min_val, max_val]">_xlfn.LAMBDA(_xlpm.number,_xlpm.min_val,_xlpm.max_val, _xldudf_LOCAL_EXEC("workbook-settings:in_range", _xlpm.number, _xlpm.min_val, _xlpm.max_val))</definedName>
-    <definedName name="JOIN_STRINGS" comment="Join two strings with a separator">_xlfn.LAMBDA(_xlpm.first_str,_xlpm.second_str,_xlpm.separator, _xldudf_LOCAL_EXEC("workbook-settings:join_strings", _xlpm.first_str, _xlpm.second_str, _xlpm.separator))</definedName>
-    <definedName name="TO_POWER" comment="Calculate power with rounding">_xlfn.LAMBDA(_xlpm.base,_xlpm.exponent,_xlpm.round_to, _xldudf_LOCAL_EXEC("workbook-settings:to_power", _xlpm.base, _xlpm.exponent, _xlpm.round_to))</definedName>
-  </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -43,7 +36,7 @@
 </file>
 
 <file path=xl/metadata.xml><?xml version="1.0" encoding="utf-8"?>
-<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xlrd="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
+<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
   <metadataTypes count="1">
     <metadataType name="XLDAPR" minSupportedVersion="120000" copy="1" pasteAll="1" pasteValues="1" merge="1" splitFirst="1" rowColShift="1" clearFormats="1" clearComments="1" assign="1" coerce="1" cellMeta="1"/>
   </metadataTypes>
@@ -491,9 +484,9 @@
       </c>
     </row>
     <row r="4" spans="2:2" x14ac:dyDescent="0.35">
-      <c r="B4" cm="1">
-        <f t="array" ref="B4">CALCULATE_AREA(2,3)</f>
-        <v>6</v>
+      <c r="B4" t="e" cm="1">
+        <f t="array" aca="1" ref="B4" ca="1">CALCULATE_AREA(2,3)</f>
+        <v>#NAME?</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
update demo sheet and functions with business_day web_page
</commit_message>
<xml_diff>
--- a/src/taskpane/utils/demo_sheet.xlsx
+++ b/src/taskpane/utils/demo_sheet.xlsx
@@ -8,12 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\brent\Code\python\src\taskpane\utils\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B4A6D8BB-0E2B-45AB-9CED-5BB807BFE7C9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8D699521-5FB4-4240-AAFC-A89F287D26F9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="16220" xr2:uid="{250729AF-73FD-4BBC-A738-7E40FF49336E}"/>
+    <workbookView xWindow="1470" yWindow="190" windowWidth="23420" windowHeight="14700" xr2:uid="{250729AF-73FD-4BBC-A738-7E40FF49336E}"/>
   </bookViews>
   <sheets>
     <sheet name="DemoFunctions" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -58,16 +59,43 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1" uniqueCount="1">
-  <si>
-    <t>Some demo sheet…</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="10">
+  <si>
+    <t>Example Functions built using Python for Excel</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> =USFEDERAL_BUSINESS_DAYS(start_date, end_date)</t>
+  </si>
+  <si>
+    <t>start_date</t>
+  </si>
+  <si>
+    <t>end_date</t>
+  </si>
+  <si>
+    <t>result</t>
+  </si>
+  <si>
+    <t>Calculate the number of business days between two dates, excluding US federal holidays.</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> =WEB_PAGE_MD(url)</t>
+  </si>
+  <si>
+    <t>url</t>
+  </si>
+  <si>
+    <t>https://www.ycombinator.com/companies/airbnb</t>
+  </si>
+  <si>
+    <t>Fetches web page content from a URL and converts to markdown.</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -75,13 +103,26 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="16"/>
+      <color theme="1"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="3" tint="0.89999084444715716"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -96,8 +137,23 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -430,66 +486,104 @@
 </a:theme>
 </file>
 
-<file path=xl/webextensions/taskpanes.xml><?xml version="1.0" encoding="utf-8"?>
-<wetp:taskpanes xmlns:wetp="http://schemas.microsoft.com/office/webextensions/taskpanes/2010/11">
-  <wetp:taskpane dockstate="right" visibility="0" width="621" row="8">
-    <wetp:webextensionref xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
-  </wetp:taskpane>
-</wetp:taskpanes>
-</file>
-
-<file path=xl/webextensions/webextension1.xml><?xml version="1.0" encoding="utf-8"?>
-<we:webextension xmlns:we="http://schemas.microsoft.com/office/webextensions/webextension/2010/11" id="{F41C696A-E33B-45FC-892B-7ACD5B532422}">
-  <we:reference id="b991da66-1687-44ee-8d65-61ab1dfd8b0f" version="1.0.0.0" store="developer" storeType="Registry"/>
-  <we:alternateReferences/>
-  <we:properties>
-    <we:property name="calculate_area" value="{&quot;name&quot;:&quot;calculate_area&quot;,&quot;signature&quot;:&quot;CALCULATE_AREA(length, width)&quot;,&quot;description&quot;:&quot;Calculate area of rectangle&quot;,&quot;code&quot;:&quot;def calculate_area(length, width):\n    \&quot;\&quot;\&quot;Calculate area of rectangle.\n    Args:\n        length (float): Length of rectangle\n        width (float): Width of rectangle\n    Returns:\n        float: Area of rectangle\n    \&quot;\&quot;\&quot;\n    return length * width\n\ntest_cases = [\n    [5, 4],      # -&gt; 20\n    [2.5, 4],    # -&gt; 10\n    [10, 10],    # -&gt; 100\n    [1, 1],      # -&gt; 1\n    [0.5, 2]     # -&gt; 1\n]\n\n# Excel usage: =CALCULATE_AREA(5, 4)&quot;,&quot;resultLine&quot;:&quot;\n\nresult = calculate_area(arg1, arg2)&quot;,&quot;formula&quot;:&quot;=LAMBDA(length, width, LOCAL.EXEC(\&quot;workbook-settings:calculate_area\&quot;, length, width))&quot;,&quot;timestamp&quot;:&quot;2025-02-10T19:05:24.194Z&quot;,&quot;uid&quot;:&quot;anonymous&quot;,&quot;excelExample&quot;:&quot;=CALCULATE_AREA(5, 4)&quot;}"/>
-    <we:property name="join_strings" value="{&quot;name&quot;:&quot;join_strings&quot;,&quot;signature&quot;:&quot;JOIN_STRINGS(first_str, second_str, separator)&quot;,&quot;description&quot;:&quot;Join two strings with a separator&quot;,&quot;code&quot;:&quot;def join_strings(first_str, second_str, separator):\n    \&quot;\&quot;\&quot;Join two strings with a separator.\n    Args:\n        first_str (str): First string\n        second_str (str): Second string\n        separator (str): Separator between strings\n    Returns:\n        str: Joined string\n    \&quot;\&quot;\&quot;\n    return f\&quot;{first_str}{separator}{second_str}\&quot;\n\ntest_cases = [\n    [\&quot;hello\&quot;, \&quot;world\&quot;, \&quot; \&quot;],      # -&gt; \&quot;hello world\&quot;\n    [\&quot;first\&quot;, \&quot;last\&quot;, \&quot;-\&quot;],       # -&gt; \&quot;first-last\&quot;\n    [\&quot;a\&quot;, \&quot;b\&quot;, \&quot;_\&quot;],             # -&gt; \&quot;a_b\&quot;\n    [\&quot;python\&quot;, \&quot;code\&quot;, \&quot;::\&quot;],     # -&gt; \&quot;python::code\&quot;\n    [\&quot;x\&quot;, \&quot;y\&quot;, \&quot;\&quot;]               # -&gt; \&quot;xy\&quot;\n]\n\n# Excel usage: =JOIN_STRINGS(\&quot;hello\&quot;, \&quot;world\&quot;, \&quot; \&quot;)&quot;,&quot;resultLine&quot;:&quot;\n\nresult = join_strings(arg1, arg2, arg3)&quot;,&quot;formula&quot;:&quot;=LAMBDA(first_str, second_str, separator, LOCAL.EXEC(\&quot;workbook-settings:join_strings\&quot;, first_str, second_str, separator))&quot;,&quot;timestamp&quot;:&quot;2025-02-10T19:05:24.258Z&quot;,&quot;uid&quot;:&quot;anonymous&quot;,&quot;excelExample&quot;:&quot;=JOIN_STRINGS(\&quot;hello\&quot;, \&quot;world\&quot;, \&quot; \&quot;)&quot;}"/>
-    <we:property name="in_range" value="{&quot;name&quot;:&quot;in_range&quot;,&quot;signature&quot;:&quot;IN_RANGE(number, min_val, max_val)&quot;,&quot;description&quot;:&quot;Check if number is in range [min_val, max_val]&quot;,&quot;code&quot;:&quot;def in_range(number, min_val, max_val):\n    \&quot;\&quot;\&quot;Check if number is in range [min_val, max_val].\n    Args:\n        number (float): Number to check\n        min_val (float): Minimum value\n        max_val (float): Maximum value\n    Returns:\n        bool: True if in range, False otherwise\n    \&quot;\&quot;\&quot;\n    return min_val &lt;= number &lt;= max_val\n\ntest_cases = [\n    [5, 0, 10],       # -&gt; True\n    [-1, 0, 100],     # -&gt; False\n    [50, 50, 50],     # -&gt; True\n    [25, 0, 20],      # -&gt; False\n    [3.14, 3, 4]      # -&gt; True\n]\n\n# Excel usage: =IN_RANGE(5, 0, 10)&quot;,&quot;resultLine&quot;:&quot;\n\nresult = in_range(arg1, arg2, arg3)&quot;,&quot;formula&quot;:&quot;=LAMBDA(number, min_val, max_val, LOCAL.EXEC(\&quot;workbook-settings:in_range\&quot;, number, min_val, max_val))&quot;,&quot;timestamp&quot;:&quot;2025-02-10T19:05:24.318Z&quot;,&quot;uid&quot;:&quot;anonymous&quot;,&quot;excelExample&quot;:&quot;=IN_RANGE(5, 0, 10)&quot;}"/>
-    <we:property name="to_power" value="{&quot;name&quot;:&quot;to_power&quot;,&quot;signature&quot;:&quot;TO_POWER(base, exponent, round_to)&quot;,&quot;description&quot;:&quot;Calculate power with rounding&quot;,&quot;code&quot;:&quot;def to_power(base, exponent, round_to):\n    \&quot;\&quot;\&quot;Calculate power with rounding.\n    Args:\n        base (float): Base number\n        exponent (float): Exponent\n        round_to (int): Decimal places to round to\n    Returns:\n        float: Result rounded to specified decimals\n    \&quot;\&quot;\&quot;\n    return round(base ** exponent, round_to)\n\ntest_cases = [\n    [2, 3, 0],        # -&gt; 8\n    [5, 2, 1],        # -&gt; 25.0\n    [3, 0.5, 2],      # -&gt; 1.73\n    [10, -1, 3],      # -&gt; 0.100\n    [2.5, 2, 2]       # -&gt; 6.25\n]\n\n# Excel usage: =TO_POWER(2, 3, 0)&quot;,&quot;resultLine&quot;:&quot;\n\nresult = to_power(arg1, arg2, arg3)&quot;,&quot;formula&quot;:&quot;=LAMBDA(base, exponent, round_to, LOCAL.EXEC(\&quot;workbook-settings:to_power\&quot;, base, exponent, round_to))&quot;,&quot;timestamp&quot;:&quot;2025-02-10T19:05:24.376Z&quot;,&quot;uid&quot;:&quot;anonymous&quot;,&quot;excelExample&quot;:&quot;=TO_POWER(2, 3, 0)&quot;}"/>
-    <we:property name="add_two_days" value="{&quot;name&quot;:&quot;add_two_days&quot;,&quot;signature&quot;:&quot;ADD_TWO_DAYS(date_input)&quot;,&quot;description&quot;:&quot;Add two days to the given date&quot;,&quot;code&quot;:&quot;def add_two_days(date_input):\n    \&quot;\&quot;\&quot;Add two days to the given date.\n    Args:\n        date_input (str or int): Date in 'YYYY-MM-DD' format or Excel serial date\n    Returns:\n        str: New date in 'YYYY-MM-DD' format\n    \&quot;\&quot;\&quot;\n    from datetime import datetime, timedelta\n    \n    if isinstance(date_input, int):\n        # Excel serial date to datetime conversion\n        date = datetime(1899, 12, 30) + timedelta(days=date_input)\n    else:\n        date = datetime.strptime(date_input, '%Y-%m-%d')\n    \n    new_date = date + timedelta(days=2)\n    return new_date.strftime('%Y-%m-%d')\n\ntest_cases = [\n    [43831],\n    [44561],\n    ['2024-06-15'],\n    ['2025-01-01']\n]\n\n# Excel usage: =ADD_TWO_DAYS(43831)&quot;,&quot;resultLine&quot;:&quot;\n\nresult = add_two_days(arg1)&quot;,&quot;formula&quot;:&quot;=LAMBDA(date_input, LOCAL.EXEC(\&quot;workbook-settings:add_two_days\&quot;, date_input))&quot;,&quot;timestamp&quot;:&quot;2025-02-10T19:05:24.436Z&quot;,&quot;uid&quot;:&quot;anonymous&quot;,&quot;excelExample&quot;:&quot;=ADD_TWO_DAYS(43831)&quot;}"/>
-  </we:properties>
-  <we:bindings/>
-  <we:snapshot xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships"/>
-  <we:extLst>
-    <a:ext xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" uri="{D87F86FE-615C-45B5-9D79-34F1136793EB}">
-      <we:containsCustomFunctions val="1"/>
-    </a:ext>
-    <a:ext xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" uri="{7C84B067-C214-45C3-A712-C9D94CD141B2}">
-      <we:customFunctionIdList>
-        <we:customFunctionIds>_xldudf_LOCAL_RUNPY</we:customFunctionIds>
-        <we:customFunctionIds>_xldudf_LOCAL_EXEC</we:customFunctionIds>
-      </we:customFunctionIdList>
-    </a:ext>
-  </we:extLst>
-</we:webextension>
-</file>
-
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C4B100FF-9D63-42FC-AE53-2720774D37AA}">
-  <dimension ref="B2:B4"/>
+  <dimension ref="A1:C13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+      <selection activeCell="B23" sqref="B23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="2" max="2" width="8.90625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="13.08984375" customWidth="1"/>
+    <col min="2" max="2" width="13.6328125" customWidth="1"/>
+    <col min="3" max="3" width="59.6328125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:2" x14ac:dyDescent="0.35">
-      <c r="B2" t="s">
+    <row r="1" spans="1:3" ht="24.5" customHeight="1" x14ac:dyDescent="0.5">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="2:2" x14ac:dyDescent="0.35">
-      <c r="B4" t="e" cm="1">
-        <f t="array" aca="1" ref="B4" ca="1">CALCULATE_AREA(2,3)</f>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A3" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="B3" s="4"/>
+      <c r="C3" s="4"/>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A4" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A6" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="B6" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="C6" s="3" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A7" s="2">
+        <v>43831</v>
+      </c>
+      <c r="B7" s="2">
+        <v>43861</v>
+      </c>
+      <c r="C7" t="e" cm="1">
+        <f t="array" aca="1" ref="C7" ca="1">USFEDERAL_BUSINESS_DAYS(A7,B7)</f>
+        <v>#NAME?</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A9" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="B9" s="4"/>
+      <c r="C9" s="4"/>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A10" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A12" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="B12" s="5"/>
+      <c r="C12" s="5" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" ht="323" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A13" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="C13" s="6" t="e" cm="1">
+        <f t="array" aca="1" ref="C13" ca="1">WEB_PAGE_MD(A13)</f>
         <v>#NAME?</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{44C8A616-AC59-49E2-B4E1-74B42C58C5C9}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
fix auth bug, remove extra sheet from demo
</commit_message>
<xml_diff>
--- a/src/taskpane/utils/demo_sheet.xlsx
+++ b/src/taskpane/utils/demo_sheet.xlsx
@@ -8,13 +8,12 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\brent\Code\python\src\taskpane\utils\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8D699521-5FB4-4240-AAFC-A89F287D26F9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{22FAD08D-3E10-441A-819E-13A2546351B4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1470" yWindow="190" windowWidth="23420" windowHeight="14700" xr2:uid="{250729AF-73FD-4BBC-A738-7E40FF49336E}"/>
+    <workbookView xWindow="1620" yWindow="430" windowWidth="23420" windowHeight="14700" xr2:uid="{250729AF-73FD-4BBC-A738-7E40FF49336E}"/>
   </bookViews>
   <sheets>
     <sheet name="DemoFunctions" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet1" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -61,9 +60,6 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="10">
   <si>
-    <t>Example Functions built using Python for Excel</t>
-  </si>
-  <si>
     <t xml:space="preserve"> =USFEDERAL_BUSINESS_DAYS(start_date, end_date)</t>
   </si>
   <si>
@@ -89,6 +85,9 @@
   </si>
   <si>
     <t>Fetches web page content from a URL and converts to markdown.</t>
+  </si>
+  <si>
+    <t>Example functions built using Boardflare Python for Excel</t>
   </si>
 </sst>
 </file>
@@ -111,7 +110,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -121,6 +120,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="3" tint="0.89999084444715716"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.79998168889431442"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -137,9 +142,8 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
@@ -154,6 +158,8 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -491,7 +497,7 @@
   <dimension ref="A1:C13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B23" sqref="B23"/>
+      <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -502,38 +508,40 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" ht="24.5" customHeight="1" x14ac:dyDescent="0.5">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="B1" s="8"/>
+      <c r="C1" s="8"/>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A3" s="3" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A3" s="4" t="s">
-        <v>1</v>
-      </c>
-      <c r="B3" s="4"/>
-      <c r="C3" s="4"/>
+      <c r="B3" s="3"/>
+      <c r="C3" s="3"/>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A6" s="3" t="s">
+      <c r="A6" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B6" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="B6" s="3" t="s">
+      <c r="C6" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="C6" s="3" t="s">
-        <v>4</v>
-      </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A7" s="2">
+      <c r="A7" s="1">
         <v>43831</v>
       </c>
-      <c r="B7" s="2">
+      <c r="B7" s="1">
         <v>43861</v>
       </c>
       <c r="C7" t="e" cm="1">
@@ -542,31 +550,31 @@
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A9" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="B9" s="4"/>
-      <c r="C9" s="4"/>
+      <c r="A9" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="B9" s="3"/>
+      <c r="C9" s="3"/>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A12" s="5" t="s">
+      <c r="A12" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="B12" s="4"/>
+      <c r="C12" s="4" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" ht="323" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A13" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="B12" s="5"/>
-      <c r="C12" s="5" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="13" spans="1:3" ht="323" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A13" s="7" t="s">
-        <v>8</v>
-      </c>
-      <c r="C13" s="6" t="e" cm="1">
+      <c r="C13" s="5" t="e" cm="1">
         <f t="array" aca="1" ref="C13" ca="1">WEB_PAGE_MD(A13)</f>
         <v>#NAME?</v>
       </c>
@@ -574,16 +582,4 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{44C8A616-AC59-49E2-B4E1-74B42C58C5C9}">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
-  <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
 </file>
</xml_diff>